<commit_message>
Learn about the maven project and created a stand alone application using maven goals
</commit_message>
<xml_diff>
--- a/Maven 07-02-2026/Guide_on_maven_proejct.xlsx
+++ b/Maven 07-02-2026/Guide_on_maven_proejct.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gyana\Desktop\Maven-pro-practice\Maven 07-02-2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD1B425F-37E8-4A0B-849A-9C940F11A573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1CCC64-5ED7-41E7-BE2D-633B7BB43181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FBED00E1-8C25-4FA9-8463-F7DF7991C011}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Serial No.</t>
   </si>
@@ -245,6 +245,111 @@
   </si>
   <si>
     <t>Folder opend in the VS Code and have our quick start application  project.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We can also use command </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">mvn package directly </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>from the begining</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> it will</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> execute the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">clean, compile, test and package </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>at a time and it will run one by one automatically. First will clear the environment and will create the target file and package it directly</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Process done automatically and created a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Target folder </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and showed </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Build success.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -648,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63273DEC-CF99-43E6-9832-A27198233AB5}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,6 +898,17 @@
         <v>21</v>
       </c>
     </row>
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>